<commit_message>
xwh: mappingbooks updated to 1004 version
</commit_message>
<xml_diff>
--- a/DbLayouts/L6-共同作業/AcAcctCheck.xlsx
+++ b/DbLayouts/L6-共同作業/AcAcctCheck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L6-共同作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021-10-19 Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C8DA62-58D3-4EEB-A992-B48D7E7A9C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE26E991-0A42-4720-9581-2AA68BDAC44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1151,36 +1151,36 @@
       <c r="A12" s="16">
         <v>4</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>48</v>
+      <c r="B12" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="34">
+        <v>73</v>
+      </c>
+      <c r="E12" s="16">
         <v>3</v>
       </c>
       <c r="F12" s="33"/>
-      <c r="G12" s="25"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>5</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" s="34">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="25"/>
@@ -1189,40 +1189,40 @@
       <c r="A14" s="16">
         <v>6</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="32">
-        <v>18</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="34">
+        <v>20</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>23</v>
+      <c r="B15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="32">
-        <v>8</v>
-      </c>
-      <c r="F15" s="33"/>
+        <v>18</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>21</v>
+      </c>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1230,10 +1230,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>32</v>
@@ -1249,10 +1249,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>32</v>
@@ -1268,10 +1268,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>32</v>
@@ -1287,20 +1287,18 @@
         <v>11</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="32">
-        <v>18</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>21</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F19" s="33"/>
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1308,10 +1306,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>32</v>
@@ -1322,17 +1320,17 @@
       <c r="F20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="23"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>13</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>32</v>
@@ -1343,96 +1341,124 @@
       <c r="F21" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>14</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="35">
-        <v>6</v>
-      </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="27"/>
+      <c r="B22" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="32">
+        <v>18</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>15</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="35"/>
+        <v>12</v>
+      </c>
+      <c r="E23" s="35">
+        <v>6</v>
+      </c>
       <c r="F23" s="35"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>16</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="35">
-        <v>6</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E24" s="35"/>
       <c r="F24" s="35"/>
-      <c r="G24" s="29"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>17</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="35"/>
+        <v>12</v>
+      </c>
+      <c r="E25" s="35">
+        <v>6</v>
+      </c>
       <c r="F25" s="35"/>
       <c r="G25" s="29"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>18</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="16">
-        <v>3</v>
-      </c>
+      <c r="B26" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="29"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1448,7 +1474,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F14 F19:F21" numberStoredAsText="1"/>
+    <ignoredError sqref="F15 F20:F22" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>